<commit_message>
Add 7-31-19 Results for Subchallenge 2
</commit_message>
<xml_diff>
--- a/Rankings.xlsx
+++ b/Rankings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colby Ford\Desktop\malaria_DREAM2019\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colbyford/Documents/malaria_DREAM2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95510475-95DA-424B-A527-1574EE196BC3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B39AEEF6-F559-454B-B9F0-E2C82D0BCB4C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{A0BB4CF1-3FD1-463D-91C5-7576C85CF853}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{A0BB4CF1-3FD1-463D-91C5-7576C85CF853}"/>
   </bookViews>
   <sheets>
     <sheet name="Rankings" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -53,12 +53,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Fast = 1, Slow = 0</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Fast = 1, Slow = 0</t>
         </r>
       </text>
     </comment>
@@ -253,15 +262,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="9"/>
-      <color indexed="81"/>
+      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
     <font>
-      <b/>
       <sz val="9"/>
-      <color indexed="81"/>
+      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -2136,12 +2145,12 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2158,7 +2167,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2176,7 +2185,7 @@
       </c>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2207,15 +2216,15 @@
       <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -2235,7 +2244,7 @@
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -2259,7 +2268,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2281,7 +2290,7 @@
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -2305,7 +2314,7 @@
       </c>
       <c r="K4" s="3"/>
     </row>
-    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2331,7 +2340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -2345,7 +2354,7 @@
         <v>1.80383143</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -2359,7 +2368,7 @@
         <v>1.9385349199999999</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -2373,7 +2382,7 @@
         <v>1.5957590800000001</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -2387,7 +2396,7 @@
         <v>1.78690711</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -2401,7 +2410,7 @@
         <v>1.65785476</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -2415,7 +2424,7 @@
         <v>1.73527947</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -2429,7 +2438,7 @@
         <v>1.8818464399999999</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -2443,7 +2452,7 @@
         <v>1.6822115200000001</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -2457,7 +2466,7 @@
         <v>1.84912298</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -2471,7 +2480,7 @@
         <v>1.7818969600000001</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -2485,7 +2494,7 @@
         <v>1.5792381600000001</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -2499,7 +2508,7 @@
         <v>1.6135952099999999</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -2513,7 +2522,7 @@
         <v>1.64111187</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -2527,7 +2536,7 @@
         <v>1.75081511</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -2541,7 +2550,7 @@
         <v>1.0556118400000001</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -2555,7 +2564,7 @@
         <v>1.7797271100000001</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -2569,7 +2578,7 @@
         <v>1.1704842200000001</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -2583,7 +2592,7 @@
         <v>1.1116242300000001</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -2597,7 +2606,7 @@
         <v>1.8061513300000001</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -2611,7 +2620,7 @@
         <v>1.73873754</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -2639,18 +2648,18 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -2667,7 +2676,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>33</v>
       </c>
@@ -2676,6 +2685,9 @@
       </c>
       <c r="C2">
         <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
       </c>
       <c r="E2">
         <f>SUM(B2:D2)</f>
@@ -2692,7 +2704,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>34</v>
       </c>
@@ -2702,9 +2714,12 @@
       <c r="C3">
         <v>1</v>
       </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
       <c r="E3">
         <f t="shared" ref="E3:E33" si="0">SUM(B3:D3)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>4</v>
@@ -2715,7 +2730,7 @@
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>35</v>
       </c>
@@ -2725,9 +2740,12 @@
       <c r="C4">
         <v>1</v>
       </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>5</v>
@@ -2740,7 +2758,7 @@
       </c>
       <c r="K4" s="3"/>
     </row>
-    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>36</v>
       </c>
@@ -2750,24 +2768,27 @@
       <c r="C5">
         <v>1</v>
       </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="4" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J5" s="4" t="e">
-        <v>#DIV/0!</v>
+      <c r="I5" s="4">
+        <v>0.46666666666666667</v>
+      </c>
+      <c r="J5" s="4">
+        <v>0.57594696646956689</v>
       </c>
       <c r="K5" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>37</v>
       </c>
@@ -2777,12 +2798,15 @@
       <c r="C6">
         <v>1</v>
       </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>38</v>
       </c>
@@ -2792,12 +2816,15 @@
       <c r="C7">
         <v>0</v>
       </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
       <c r="E7">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>39</v>
       </c>
@@ -2807,12 +2834,15 @@
       <c r="C8">
         <v>0</v>
       </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>40</v>
       </c>
@@ -2821,13 +2851,16 @@
       </c>
       <c r="C9">
         <v>1</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>41</v>
       </c>
@@ -2837,12 +2870,15 @@
       <c r="C10">
         <v>1</v>
       </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>42</v>
       </c>
@@ -2852,12 +2888,15 @@
       <c r="C11">
         <v>0</v>
       </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
       <c r="E11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>43</v>
       </c>
@@ -2867,12 +2906,15 @@
       <c r="C12">
         <v>0</v>
       </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
       <c r="E12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>44</v>
       </c>
@@ -2882,12 +2924,15 @@
       <c r="C13">
         <v>1</v>
       </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>45</v>
       </c>
@@ -2897,12 +2942,15 @@
       <c r="C14">
         <v>1</v>
       </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>46</v>
       </c>
@@ -2912,12 +2960,15 @@
       <c r="C15">
         <v>0</v>
       </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
       <c r="E15">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>47</v>
       </c>
@@ -2926,13 +2977,16 @@
       </c>
       <c r="C16">
         <v>1</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
       </c>
       <c r="E16">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>48</v>
       </c>
@@ -2942,12 +2996,15 @@
       <c r="C17">
         <v>0</v>
       </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
       <c r="E17">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>49</v>
       </c>
@@ -2957,12 +3014,15 @@
       <c r="C18">
         <v>0</v>
       </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
       <c r="E18">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>7</v>
       </c>
@@ -2972,12 +3032,15 @@
       <c r="C19">
         <v>0</v>
       </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
       <c r="E19">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>8</v>
       </c>
@@ -2987,12 +3050,15 @@
       <c r="C20">
         <v>0</v>
       </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
       <c r="E20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>11</v>
       </c>
@@ -3002,12 +3068,15 @@
       <c r="C21">
         <v>0</v>
       </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
       <c r="E21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>14</v>
       </c>
@@ -3017,12 +3086,15 @@
       <c r="C22">
         <v>1</v>
       </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
       <c r="E22">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>15</v>
       </c>
@@ -3032,12 +3104,15 @@
       <c r="C23">
         <v>0</v>
       </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
       <c r="E23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>16</v>
       </c>
@@ -3047,12 +3122,15 @@
       <c r="C24">
         <v>0</v>
       </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
       <c r="E24">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>18</v>
       </c>
@@ -3062,12 +3140,15 @@
       <c r="C25">
         <v>0</v>
       </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
       <c r="E25">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>19</v>
       </c>
@@ -3076,13 +3157,16 @@
       </c>
       <c r="C26">
         <v>1</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
       </c>
       <c r="E26">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>20</v>
       </c>
@@ -3092,12 +3176,15 @@
       <c r="C27">
         <v>1</v>
       </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
       <c r="E27">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>22</v>
       </c>
@@ -3107,12 +3194,15 @@
       <c r="C28">
         <v>1</v>
       </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
       <c r="E28">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>23</v>
       </c>
@@ -3121,13 +3211,16 @@
       </c>
       <c r="C29">
         <v>1</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
       </c>
       <c r="E29">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>26</v>
       </c>
@@ -3137,12 +3230,15 @@
       <c r="C30">
         <v>0</v>
       </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
       <c r="E30">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>27</v>
       </c>
@@ -3152,12 +3248,15 @@
       <c r="C31">
         <v>1</v>
       </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
       <c r="E31">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>29</v>
       </c>
@@ -3167,12 +3266,15 @@
       <c r="C32">
         <v>0</v>
       </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
       <c r="E32">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>30</v>
       </c>
@@ -3182,12 +3284,27 @@
       <c r="C33">
         <v>1</v>
       </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
       <c r="E33">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="E2:E33">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>

</xml_diff>